<commit_message>
add short relatedArtifact 19cf965c645e89023c73f15d58ad39f776d87859
</commit_message>
<xml_diff>
--- a/ig/sd-add-short-relatedArtifact/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-add-short-relatedArtifact/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-11T10:01:52+00:00</t>
+    <t>2024-01-11T10:11:59+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1475,7 +1475,7 @@
 </t>
   </si>
   <si>
-    <t>References and dependencies</t>
+    <t>Publications et réumé des résultats / Publications about the study and Summary results</t>
   </si>
   <si>
     <t>Citations, references and other related documents.</t>
@@ -10341,7 +10341,7 @@
         <v>79</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>80</v>

</xml_diff>